<commit_message>
Update thong tin db
</commit_message>
<xml_diff>
--- a/Tai_Lieu_(VN)/Thông tin chung - CONTEC.xlsx
+++ b/Tai_Lieu_(VN)/Thông tin chung - CONTEC.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thach\Desktop\CONTEC_Migration\PG\Tai_Lieu_(VN)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thach\Desktop\CONTEC_Migration\Tai_Lieu_(VN)\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20325" windowHeight="7080"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20325" windowHeight="7080" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Các bước chuyển đổi" sheetId="2" r:id="rId1"/>
@@ -134,12 +134,6 @@
     <t>user: CNT_USR1</t>
   </si>
   <si>
-    <t>tns: CONORCL</t>
-  </si>
-  <si>
-    <t>pass: CNT_USR1P</t>
-  </si>
-  <si>
     <t>【補足】FJグループの方でFJ-WAN経由で接続したい場合は以下の社内URLを参考にして頂く事で接続可能です。</t>
     <rPh sb="1" eb="3">
       <t>ホソク</t>
@@ -255,6 +249,12 @@
   </si>
   <si>
     <t>8/ Build hết lỗi và F5 Run chạy được màn hình  --&gt;   (Tiến độ là 30%)</t>
+  </si>
+  <si>
+    <t>tns: CNT_USR1</t>
+  </si>
+  <si>
+    <t>pass: DEV02</t>
   </si>
 </sst>
 </file>
@@ -2534,7 +2534,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:B35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
@@ -2626,7 +2626,7 @@
     </row>
     <row r="23" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B23" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2637,7 +2637,7 @@
     </row>
     <row r="26" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -2687,7 +2687,7 @@
   <sheetData>
     <row r="2" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -3289,7 +3289,7 @@
     </row>
     <row r="32" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -3871,7 +3871,7 @@
     </row>
     <row r="61" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B61" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
@@ -4393,7 +4393,7 @@
     </row>
     <row r="87" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B87" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C87" s="1"/>
       <c r="D87" s="1"/>
@@ -4995,7 +4995,7 @@
     </row>
     <row r="117" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B117" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C117" s="1"/>
       <c r="D117" s="1"/>
@@ -5697,7 +5697,7 @@
     </row>
     <row r="152" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B152" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C152" s="1"/>
       <c r="D152" s="1"/>
@@ -6119,10 +6119,10 @@
     </row>
     <row r="173" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B173" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D173" s="1"/>
       <c r="E173" s="1"/>
@@ -6144,7 +6144,7 @@
     <row r="174" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B174" s="1"/>
       <c r="C174" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D174" s="1"/>
       <c r="E174" s="1"/>
@@ -6166,7 +6166,7 @@
     <row r="175" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B175" s="1"/>
       <c r="C175" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D175" s="1"/>
       <c r="E175" s="1"/>
@@ -6188,7 +6188,7 @@
     <row r="176" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B176" s="1"/>
       <c r="C176" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D176" s="1"/>
       <c r="E176" s="1"/>
@@ -6609,7 +6609,7 @@
     </row>
     <row r="197" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B197" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C197" s="1"/>
       <c r="D197" s="1"/>
@@ -7031,7 +7031,7 @@
     </row>
     <row r="218" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B218" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C218" s="1"/>
       <c r="D218" s="1"/>
@@ -7633,7 +7633,7 @@
     </row>
     <row r="248" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B248" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C248" s="1"/>
       <c r="D248" s="1"/>
@@ -7655,7 +7655,7 @@
     </row>
     <row r="249" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B249" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C249" s="1"/>
       <c r="D249" s="1"/>
@@ -8057,7 +8057,7 @@
     </row>
     <row r="269" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B269" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C269" s="1"/>
       <c r="D269" s="1"/>
@@ -8639,7 +8639,7 @@
     </row>
     <row r="298" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B298" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C298" s="1"/>
       <c r="D298" s="1"/>
@@ -9241,7 +9241,7 @@
     </row>
     <row r="328" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B328" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C328" s="1"/>
       <c r="D328" s="1"/>
@@ -9803,7 +9803,7 @@
     </row>
     <row r="356" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B356" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C356" s="1"/>
       <c r="D356" s="1"/>
@@ -9825,7 +9825,7 @@
     </row>
     <row r="357" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B357" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C357" s="1"/>
       <c r="D357" s="1"/>
@@ -9847,7 +9847,7 @@
     </row>
     <row r="358" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B358" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C358" s="1"/>
       <c r="D358" s="1"/>
@@ -9909,7 +9909,7 @@
     </row>
     <row r="361" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B361" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C361" s="1"/>
       <c r="D361" s="1"/>
@@ -12636,8 +12636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I25" sqref="I25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12649,12 +12649,12 @@
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>36</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sheet add file batch
</commit_message>
<xml_diff>
--- a/Tai_Lieu_(VN)/Thông tin chung - CONTEC.xlsx
+++ b/Tai_Lieu_(VN)/Thông tin chung - CONTEC.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thach\Desktop\CONTEC_Migration\Tai_Lieu_(VN)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\CONTEC_Migration\Tai_Lieu_(VN)\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20325" windowHeight="7080" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20325" windowHeight="7080" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Các bước chuyển đổi" sheetId="2" r:id="rId1"/>
     <sheet name="Setup môi trường" sheetId="4" r:id="rId2"/>
     <sheet name="Tk login vào máy Remote" sheetId="1" r:id="rId3"/>
     <sheet name="Thông tin kết nối DB" sheetId="3" r:id="rId4"/>
+    <sheet name="file Batch" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>cis07@ad.fjazure.com</t>
   </si>
@@ -255,6 +256,12 @@
   </si>
   <si>
     <t>tns: DEV02</t>
+  </si>
+  <si>
+    <t>copy exe vào =&gt; \\jobsvr01\c\CRAFT\JOB\CNT\PRG\EXE</t>
+  </si>
+  <si>
+    <t>copy bat vào =&gt; E:\CRAFT\CVT起動用バッチ</t>
   </si>
 </sst>
 </file>
@@ -2696,8 +2703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:S491"/>
   <sheetViews>
-    <sheetView topLeftCell="A151" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView topLeftCell="A322" workbookViewId="0">
+      <selection activeCell="B249" sqref="B249"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12557,7 +12564,7 @@
   <dimension ref="C3:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12653,7 +12660,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
@@ -12689,4 +12696,29 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O23" sqref="O23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update thông tin chung
</commit_message>
<xml_diff>
--- a/Tai_Lieu_(VN)/Thông tin chung - CONTEC.xlsx
+++ b/Tai_Lieu_(VN)/Thông tin chung - CONTEC.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\CONTEC_Migration\Tai_Lieu_(VN)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thach\Desktop\CONTEC_Migration\Tai_Lieu_(VN)\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20325" windowHeight="7080" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20325" windowHeight="7080"/>
   </bookViews>
   <sheets>
     <sheet name="Các bước chuyển đổi" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t>cis07@ad.fjazure.com</t>
   </si>
@@ -118,9 +118,6 @@
   </si>
   <si>
     <t>3/ "CLTIDCONTEC  "</t>
-  </si>
-  <si>
-    <t>9/ Bấm từng nút ở phía trên F1-F12 và fix lỗi (tham khảo source mẫu)</t>
   </si>
   <si>
     <t>10/ Bấm từng F1-F12 và fix lỗi (tham khảo source mẫu)</t>
@@ -263,12 +260,21 @@
   <si>
     <t>copy bat vào =&gt; E:\CRAFT\CVT起動用バッチ</t>
   </si>
+  <si>
+    <t xml:space="preserve">9/ Bấm từng nút ở phía trên F1-F12 và fix lỗi (tham khảo source mẫu) </t>
+  </si>
+  <si>
+    <t>(Các nút trên màn hình đều phải hoạt động )</t>
+  </si>
+  <si>
+    <t>Mọi người cho CHIỀU CAO    của BUTTON , LABEL bà TEXTBOX  đều là 22 thì sẽ đều và đẹp nhé !! (label, textbox thì cho Multiline = true  sẽ chỉnh dc)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -322,6 +328,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -344,7 +358,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -355,6 +369,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2556,10 +2571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:B35"/>
+  <dimension ref="B3:B37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P27" sqref="P27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2610,87 +2625,97 @@
       </c>
     </row>
     <row r="14" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B14" s="4"/>
+      <c r="B14" s="8" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="15" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="4"/>
+    </row>
+    <row r="16" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B16" s="4"/>
-    </row>
     <row r="17" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="4"/>
+    </row>
+    <row r="18" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B18" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="4"/>
-    </row>
     <row r="19" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="4"/>
+    </row>
+    <row r="20" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B20" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B20" s="5" t="s">
+    <row r="21" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B21" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="5" t="s">
+    <row r="22" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B22" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B22" s="5" t="s">
+    <row r="23" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B23" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="5" t="s">
+    <row r="24" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B24" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B25" s="4"/>
+    </row>
+    <row r="26" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B26" s="4"/>
+    </row>
+    <row r="27" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B27" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="4"/>
-    </row>
-    <row r="25" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="4"/>
-    </row>
-    <row r="26" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B26" s="4" t="s">
-        <v>58</v>
+    <row r="28" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B28" s="4"/>
+    </row>
+    <row r="29" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B29" s="4" t="s">
+        <v>62</v>
       </c>
     </row>
-    <row r="27" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B27" s="4"/>
-    </row>
-    <row r="28" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B28" s="4" t="s">
+    <row r="30" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B30" s="8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B31" s="4"/>
+    </row>
+    <row r="32" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B32" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B29" s="4"/>
-    </row>
-    <row r="30" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B30" s="4" t="s">
+    <row r="33" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B33" s="4"/>
+    </row>
+    <row r="34" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B34" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B31" s="4"/>
-    </row>
-    <row r="32" spans="2:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B32" s="4" t="s">
+    <row r="37" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B37" s="3" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B35" s="3" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -2711,7 +2736,7 @@
   <sheetData>
     <row r="2" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
@@ -3313,7 +3338,7 @@
     </row>
     <row r="32" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -3895,7 +3920,7 @@
     </row>
     <row r="61" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B61" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
@@ -4417,7 +4442,7 @@
     </row>
     <row r="87" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B87" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C87" s="1"/>
       <c r="D87" s="1"/>
@@ -5019,7 +5044,7 @@
     </row>
     <row r="117" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B117" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C117" s="1"/>
       <c r="D117" s="1"/>
@@ -5721,7 +5746,7 @@
     </row>
     <row r="152" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B152" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C152" s="1"/>
       <c r="D152" s="1"/>
@@ -6143,10 +6168,10 @@
     </row>
     <row r="173" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B173" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D173" s="1"/>
       <c r="E173" s="1"/>
@@ -6168,7 +6193,7 @@
     <row r="174" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B174" s="1"/>
       <c r="C174" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D174" s="1"/>
       <c r="E174" s="1"/>
@@ -6190,7 +6215,7 @@
     <row r="175" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B175" s="1"/>
       <c r="C175" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D175" s="1"/>
       <c r="E175" s="1"/>
@@ -6212,7 +6237,7 @@
     <row r="176" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B176" s="1"/>
       <c r="C176" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D176" s="1"/>
       <c r="E176" s="1"/>
@@ -6633,7 +6658,7 @@
     </row>
     <row r="197" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B197" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C197" s="1"/>
       <c r="D197" s="1"/>
@@ -7055,7 +7080,7 @@
     </row>
     <row r="218" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B218" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C218" s="1"/>
       <c r="D218" s="1"/>
@@ -7657,7 +7682,7 @@
     </row>
     <row r="248" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B248" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C248" s="1"/>
       <c r="D248" s="1"/>
@@ -7679,7 +7704,7 @@
     </row>
     <row r="249" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B249" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C249" s="1"/>
       <c r="D249" s="1"/>
@@ -8081,7 +8106,7 @@
     </row>
     <row r="269" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B269" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C269" s="1"/>
       <c r="D269" s="1"/>
@@ -8663,7 +8688,7 @@
     </row>
     <row r="298" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B298" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C298" s="1"/>
       <c r="D298" s="1"/>
@@ -9265,7 +9290,7 @@
     </row>
     <row r="328" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B328" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C328" s="1"/>
       <c r="D328" s="1"/>
@@ -9827,7 +9852,7 @@
     </row>
     <row r="356" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B356" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C356" s="1"/>
       <c r="D356" s="1"/>
@@ -9849,7 +9874,7 @@
     </row>
     <row r="357" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B357" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C357" s="1"/>
       <c r="D357" s="1"/>
@@ -9871,7 +9896,7 @@
     </row>
     <row r="358" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B358" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C358" s="1"/>
       <c r="D358" s="1"/>
@@ -9933,7 +9958,7 @@
     </row>
     <row r="361" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B361" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C361" s="1"/>
       <c r="D361" s="1"/>
@@ -12668,7 +12693,7 @@
   <sheetData>
     <row r="3" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B3" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" s="6"/>
     </row>
@@ -12678,7 +12703,7 @@
     </row>
     <row r="5" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B5" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C5" s="6"/>
     </row>
@@ -12688,7 +12713,7 @@
     </row>
     <row r="7" spans="2:3" ht="21" x14ac:dyDescent="0.35">
       <c r="B7" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C7" s="6"/>
     </row>
@@ -12702,7 +12727,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="O23" sqref="O23"/>
     </sheetView>
   </sheetViews>
@@ -12710,12 +12735,12 @@
   <sheetData>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>